<commit_message>
complete Community CRUD. add communityEdit~.
</commit_message>
<xml_diff>
--- a/sql/더미데이터만들기.xlsx
+++ b/sql/더미데이터만들기.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\jsp-team-project-in-choongang\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E12CE92-BD57-49F9-9332-0794FBC7F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36D515F-8484-4A3E-BC75-025E9C4B3BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="2520" windowWidth="24765" windowHeight="12915" xr2:uid="{0BB40357-846B-45EB-B4C9-59F5046CF9DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="4">
   <si>
     <t>INSERT INTO board VALUES(001,</t>
   </si>
@@ -34,14 +34,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,</t>
+    <t>,1,1);</t>
   </si>
   <si>
-    <t>,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,1,1);</t>
+    <t>,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,</t>
   </si>
 </sst>
 </file>
@@ -407,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1377E80-2856-4818-A189-DC42E2F95B4E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F1:F49"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -431,11 +427,11 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1" t="str">
         <f>A1&amp;B1&amp;C1&amp;D1&amp;E1</f>
-        <v>INSERT INTO board VALUES(001,12,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,12,1,1);</v>
+        <v>INSERT INTO board VALUES(001,12,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,12,1,1);</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -452,11 +448,11 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F49" si="0">A2&amp;B2&amp;C2&amp;D2&amp;E2</f>
-        <v>INSERT INTO board VALUES(001,13,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,13,1,1);</v>
+        <v>INSERT INTO board VALUES(001,13,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,13,1,1);</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -467,17 +463,17 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,14,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,14,1,1);</v>
+        <v>INSERT INTO board VALUES(001,14,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,14,1,1);</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -488,17 +484,17 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,15,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,15,1,1);</v>
+        <v>INSERT INTO board VALUES(001,15,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,15,1,1);</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -509,17 +505,17 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,16,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,16,1,1);</v>
+        <v>INSERT INTO board VALUES(001,16,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,16,1,1);</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -530,17 +526,17 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,17,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,17,1,1);</v>
+        <v>INSERT INTO board VALUES(001,17,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,17,1,1);</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -551,17 +547,17 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,18,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,18,1,1);</v>
+        <v>INSERT INTO board VALUES(001,18,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,18,1,1);</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -572,17 +568,17 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,19,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,19,1,1);</v>
+        <v>INSERT INTO board VALUES(001,19,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,19,1,1);</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -593,17 +589,17 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,20,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,20,1,1);</v>
+        <v>INSERT INTO board VALUES(001,20,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,20,1,1);</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -614,17 +610,17 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,21,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,21,1,1);</v>
+        <v>INSERT INTO board VALUES(001,21,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,21,1,1);</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,17 +631,17 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,22,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,22,1,1);</v>
+        <v>INSERT INTO board VALUES(001,22,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,22,1,1);</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -656,17 +652,17 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,23,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,23,1,1);</v>
+        <v>INSERT INTO board VALUES(001,23,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,23,1,1);</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,17 +673,17 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,24,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,24,1,1);</v>
+        <v>INSERT INTO board VALUES(001,24,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,24,1,1);</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -698,17 +694,17 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,25,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,25,1,1);</v>
+        <v>INSERT INTO board VALUES(001,25,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,25,1,1);</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -719,17 +715,17 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,26,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,26,1,1);</v>
+        <v>INSERT INTO board VALUES(001,26,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,26,1,1);</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -740,17 +736,17 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,27,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,27,1,1);</v>
+        <v>INSERT INTO board VALUES(001,27,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,27,1,1);</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -761,17 +757,17 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,28,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,28,1,1);</v>
+        <v>INSERT INTO board VALUES(001,28,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,28,1,1);</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -782,17 +778,17 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,29,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,29,1,1);</v>
+        <v>INSERT INTO board VALUES(001,29,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,29,1,1);</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -803,17 +799,17 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,30,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,30,1,1);</v>
+        <v>INSERT INTO board VALUES(001,30,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,30,1,1);</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -824,17 +820,17 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,31,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,31,1,1);</v>
+        <v>INSERT INTO board VALUES(001,31,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,31,1,1);</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -845,17 +841,17 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21">
         <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,32,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,32,1,1);</v>
+        <v>INSERT INTO board VALUES(001,32,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,32,1,1);</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -866,17 +862,17 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,33,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,33,1,1);</v>
+        <v>INSERT INTO board VALUES(001,33,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,33,1,1);</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -887,17 +883,17 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,34,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,34,1,1);</v>
+        <v>INSERT INTO board VALUES(001,34,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,34,1,1);</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -908,17 +904,17 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24">
         <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,35,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,35,1,1);</v>
+        <v>INSERT INTO board VALUES(001,35,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,35,1,1);</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -929,17 +925,17 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25">
         <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,36,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,36,1,1);</v>
+        <v>INSERT INTO board VALUES(001,36,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,36,1,1);</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -950,17 +946,17 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26">
         <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,37,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,37,1,1);</v>
+        <v>INSERT INTO board VALUES(001,37,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,37,1,1);</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,17 +967,17 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,38,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,38,1,1);</v>
+        <v>INSERT INTO board VALUES(001,38,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,38,1,1);</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -992,17 +988,17 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,39,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,39,1,1);</v>
+        <v>INSERT INTO board VALUES(001,39,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,39,1,1);</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1013,17 +1009,17 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,40,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,40,1,1);</v>
+        <v>INSERT INTO board VALUES(001,40,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,40,1,1);</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1034,17 +1030,17 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,41,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,41,1,1);</v>
+        <v>INSERT INTO board VALUES(001,41,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,41,1,1);</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1055,17 +1051,17 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,42,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,42,1,1);</v>
+        <v>INSERT INTO board VALUES(001,42,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,42,1,1);</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1076,17 +1072,17 @@
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,43,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,43,1,1);</v>
+        <v>INSERT INTO board VALUES(001,43,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,43,1,1);</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,17 +1093,17 @@
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33">
         <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,44,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,44,1,1);</v>
+        <v>INSERT INTO board VALUES(001,44,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,44,1,1);</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1118,17 +1114,17 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34">
         <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,45,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,45,1,1);</v>
+        <v>INSERT INTO board VALUES(001,45,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,45,1,1);</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1139,17 +1135,17 @@
         <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,46,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,46,1,1);</v>
+        <v>INSERT INTO board VALUES(001,46,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,46,1,1);</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1160,17 +1156,17 @@
         <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
         <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,47,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,47,1,1);</v>
+        <v>INSERT INTO board VALUES(001,47,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,47,1,1);</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1181,17 +1177,17 @@
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37">
         <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,48,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,48,1,1);</v>
+        <v>INSERT INTO board VALUES(001,48,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,48,1,1);</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1202,17 +1198,17 @@
         <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38">
         <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,49,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,49,1,1);</v>
+        <v>INSERT INTO board VALUES(001,49,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,49,1,1);</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1223,17 +1219,17 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39">
         <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,50,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,50,1,1);</v>
+        <v>INSERT INTO board VALUES(001,50,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,50,1,1);</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1244,17 +1240,17 @@
         <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40">
         <v>51</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,51,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,51,1,1);</v>
+        <v>INSERT INTO board VALUES(001,51,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,51,1,1);</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1265,17 +1261,17 @@
         <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41">
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,52,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,52,1,1);</v>
+        <v>INSERT INTO board VALUES(001,52,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,52,1,1);</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1286,17 +1282,17 @@
         <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42">
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,53,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,53,1,1);</v>
+        <v>INSERT INTO board VALUES(001,53,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,53,1,1);</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1307,17 +1303,17 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43">
         <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,54,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,54,1,1);</v>
+        <v>INSERT INTO board VALUES(001,54,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,54,1,1);</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1328,17 +1324,17 @@
         <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
         <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,55,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,55,1,1);</v>
+        <v>INSERT INTO board VALUES(001,55,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,55,1,1);</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1349,17 +1345,17 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D45">
         <v>56</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,56,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,56,1,1);</v>
+        <v>INSERT INTO board VALUES(001,56,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,56,1,1);</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1370,17 +1366,17 @@
         <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46">
         <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,57,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,57,1,1);</v>
+        <v>INSERT INTO board VALUES(001,57,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,57,1,1);</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1391,17 +1387,17 @@
         <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47">
         <v>58</v>
       </c>
       <c r="E47" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,58,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,58,1,1);</v>
+        <v>INSERT INTO board VALUES(001,58,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,58,1,1);</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1412,17 +1408,17 @@
         <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48">
         <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,59,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,59,1,1);</v>
+        <v>INSERT INTO board VALUES(001,59,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,59,1,1);</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1433,17 +1429,17 @@
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49">
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO board VALUES(001,60,'ino22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,60,1,1);</v>
+        <v>INSERT INTO board VALUES(001,60,'iin22','더미용','냉무',null,0,TO_DATE('2021-08-29 00:00:30','YYYY-MM-DD HH24:MI:SS'),'#연봉',0,null,60,1,1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>